<commit_message>
Update design documents. -Update sequence class of brake, rotate, and velocity to update. -Update pictures of upper diagram.
</commit_message>
<xml_diff>
--- a/dev/doc/sequence_design.xlsx
+++ b/dev/doc/sequence_design.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>○</t>
     <phoneticPr fontId="2"/>
@@ -807,14 +807,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>コマンドコード</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>0x10</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>データ(値)</t>
     <rPh sb="4" eb="5">
       <t>アタイ</t>
@@ -826,64 +818,64 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>1～2</t>
+    <t>チェックサム(対象範囲：0～5バイト目)</t>
+    <rPh sb="7" eb="9">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ハンイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>メ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>3～4</t>
+    <t>回転数(RPM単位) / リトルエンディアン</t>
+    <rPh sb="0" eb="3">
+      <t>カイテンスウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>タンイ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>5～6</t>
+    <t>速度(km/h、小数部分) / リトルエンディアン</t>
+    <rPh sb="0" eb="2">
+      <t>ソクド</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ショウスウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ブブン</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>チェックサム(対象範囲：0～5バイト目)</t>
-    <rPh sb="7" eb="9">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ハンイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>メ</t>
+    <t>速度(km/h、整数部分) / リトルエンディアン</t>
+    <rPh sb="0" eb="2">
+      <t>ソクド</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セイスウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ブブン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>回転数(整数部分 / RPM単位) / リトルエンディアン</t>
-    <rPh sb="0" eb="3">
-      <t>カイテンスウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>セイスウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ブブン</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>タンイ</t>
-    </rPh>
+    <t>0～1</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>回転数(小数部分 / RPM単位) / リトルエンディアン</t>
-    <rPh sb="0" eb="3">
-      <t>カイテンスウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ショウスウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ブブン</t>
-    </rPh>
+    <t>2～3</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>速度(km/h) / リトルエンディアン</t>
-    <rPh sb="0" eb="2">
-      <t>ソクド</t>
-    </rPh>
+    <t>4～5</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -936,7 +928,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1076,51 +1068,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -1208,7 +1155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1220,34 +1167,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1256,12 +1185,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2716,18 +2652,18 @@
     <xdr:to>
       <xdr:col>70</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>40521</xdr:rowOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>12121</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPr id="5" name="図 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2741,7 +2677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="762000" y="3048000"/>
-          <a:ext cx="10058400" cy="6288921"/>
+          <a:ext cx="10058400" cy="5955721"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2765,12 +2701,12 @@
     <xdr:to>
       <xdr:col>71</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>33607</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38507</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="図 3"/>
+        <xdr:cNvPr id="2" name="図 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2790,7 +2726,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="762000" y="2286000"/>
-          <a:ext cx="10058400" cy="5367607"/>
+          <a:ext cx="10058400" cy="5677307"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5467,7 +5403,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:BT82"/>
+  <dimension ref="B2:BT79"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -8401,221 +8337,97 @@
       <c r="BT59" s="7"/>
     </row>
     <row r="60" spans="4:72" x14ac:dyDescent="0.2">
-      <c r="E60" s="5"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-      <c r="M60" s="6"/>
-      <c r="N60" s="6"/>
-      <c r="O60" s="6"/>
-      <c r="P60" s="6"/>
-      <c r="Q60" s="6"/>
-      <c r="R60" s="6"/>
-      <c r="S60" s="6"/>
-      <c r="T60" s="6"/>
-      <c r="U60" s="6"/>
-      <c r="V60" s="6"/>
-      <c r="W60" s="6"/>
-      <c r="X60" s="6"/>
-      <c r="Y60" s="6"/>
-      <c r="Z60" s="6"/>
-      <c r="AA60" s="6"/>
-      <c r="AB60" s="6"/>
-      <c r="AC60" s="6"/>
-      <c r="AD60" s="6"/>
-      <c r="AE60" s="6"/>
-      <c r="AF60" s="6"/>
-      <c r="AG60" s="6"/>
-      <c r="AH60" s="6"/>
-      <c r="AI60" s="6"/>
-      <c r="AJ60" s="6"/>
-      <c r="AK60" s="6"/>
-      <c r="AL60" s="6"/>
-      <c r="AM60" s="6"/>
-      <c r="AN60" s="6"/>
-      <c r="AO60" s="6"/>
-      <c r="AP60" s="6"/>
-      <c r="AQ60" s="6"/>
-      <c r="AR60" s="6"/>
-      <c r="AS60" s="6"/>
-      <c r="AT60" s="6"/>
-      <c r="AU60" s="6"/>
-      <c r="AV60" s="6"/>
-      <c r="AW60" s="6"/>
-      <c r="AX60" s="6"/>
-      <c r="AY60" s="6"/>
-      <c r="AZ60" s="6"/>
-      <c r="BA60" s="6"/>
-      <c r="BB60" s="6"/>
-      <c r="BC60" s="6"/>
-      <c r="BD60" s="6"/>
-      <c r="BE60" s="6"/>
-      <c r="BF60" s="6"/>
-      <c r="BG60" s="6"/>
-      <c r="BH60" s="6"/>
-      <c r="BI60" s="6"/>
-      <c r="BJ60" s="6"/>
-      <c r="BK60" s="6"/>
-      <c r="BL60" s="6"/>
-      <c r="BM60" s="6"/>
-      <c r="BN60" s="6"/>
-      <c r="BO60" s="6"/>
-      <c r="BP60" s="6"/>
-      <c r="BQ60" s="6"/>
-      <c r="BR60" s="6"/>
-      <c r="BS60" s="6"/>
-      <c r="BT60" s="7"/>
-    </row>
-    <row r="61" spans="4:72" x14ac:dyDescent="0.2">
-      <c r="E61" s="5"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
-      <c r="P61" s="6"/>
-      <c r="Q61" s="6"/>
-      <c r="R61" s="6"/>
-      <c r="S61" s="6"/>
-      <c r="T61" s="6"/>
-      <c r="U61" s="6"/>
-      <c r="V61" s="6"/>
-      <c r="W61" s="6"/>
-      <c r="X61" s="6"/>
-      <c r="Y61" s="6"/>
-      <c r="Z61" s="6"/>
-      <c r="AA61" s="6"/>
-      <c r="AB61" s="6"/>
-      <c r="AC61" s="6"/>
-      <c r="AD61" s="6"/>
-      <c r="AE61" s="6"/>
-      <c r="AF61" s="6"/>
-      <c r="AG61" s="6"/>
-      <c r="AH61" s="6"/>
-      <c r="AI61" s="6"/>
-      <c r="AJ61" s="6"/>
-      <c r="AK61" s="6"/>
-      <c r="AL61" s="6"/>
-      <c r="AM61" s="6"/>
-      <c r="AN61" s="6"/>
-      <c r="AO61" s="6"/>
-      <c r="AP61" s="6"/>
-      <c r="AQ61" s="6"/>
-      <c r="AR61" s="6"/>
-      <c r="AS61" s="6"/>
-      <c r="AT61" s="6"/>
-      <c r="AU61" s="6"/>
-      <c r="AV61" s="6"/>
-      <c r="AW61" s="6"/>
-      <c r="AX61" s="6"/>
-      <c r="AY61" s="6"/>
-      <c r="AZ61" s="6"/>
-      <c r="BA61" s="6"/>
-      <c r="BB61" s="6"/>
-      <c r="BC61" s="6"/>
-      <c r="BD61" s="6"/>
-      <c r="BE61" s="6"/>
-      <c r="BF61" s="6"/>
-      <c r="BG61" s="6"/>
-      <c r="BH61" s="6"/>
-      <c r="BI61" s="6"/>
-      <c r="BJ61" s="6"/>
-      <c r="BK61" s="6"/>
-      <c r="BL61" s="6"/>
-      <c r="BM61" s="6"/>
-      <c r="BN61" s="6"/>
-      <c r="BO61" s="6"/>
-      <c r="BP61" s="6"/>
-      <c r="BQ61" s="6"/>
-      <c r="BR61" s="6"/>
-      <c r="BS61" s="6"/>
-      <c r="BT61" s="7"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
+      <c r="R60" s="9"/>
+      <c r="S60" s="9"/>
+      <c r="T60" s="9"/>
+      <c r="U60" s="9"/>
+      <c r="V60" s="9"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
+      <c r="Y60" s="9"/>
+      <c r="Z60" s="9"/>
+      <c r="AA60" s="9"/>
+      <c r="AB60" s="9"/>
+      <c r="AC60" s="9"/>
+      <c r="AD60" s="9"/>
+      <c r="AE60" s="9"/>
+      <c r="AF60" s="9"/>
+      <c r="AG60" s="9"/>
+      <c r="AH60" s="9"/>
+      <c r="AI60" s="9"/>
+      <c r="AJ60" s="9"/>
+      <c r="AK60" s="9"/>
+      <c r="AL60" s="9"/>
+      <c r="AM60" s="9"/>
+      <c r="AN60" s="9"/>
+      <c r="AO60" s="9"/>
+      <c r="AP60" s="9"/>
+      <c r="AQ60" s="9"/>
+      <c r="AR60" s="9"/>
+      <c r="AS60" s="9"/>
+      <c r="AT60" s="9"/>
+      <c r="AU60" s="9"/>
+      <c r="AV60" s="9"/>
+      <c r="AW60" s="9"/>
+      <c r="AX60" s="9"/>
+      <c r="AY60" s="9"/>
+      <c r="AZ60" s="9"/>
+      <c r="BA60" s="9"/>
+      <c r="BB60" s="9"/>
+      <c r="BC60" s="9"/>
+      <c r="BD60" s="9"/>
+      <c r="BE60" s="9"/>
+      <c r="BF60" s="9"/>
+      <c r="BG60" s="9"/>
+      <c r="BH60" s="9"/>
+      <c r="BI60" s="9"/>
+      <c r="BJ60" s="9"/>
+      <c r="BK60" s="9"/>
+      <c r="BL60" s="9"/>
+      <c r="BM60" s="9"/>
+      <c r="BN60" s="9"/>
+      <c r="BO60" s="9"/>
+      <c r="BP60" s="9"/>
+      <c r="BQ60" s="9"/>
+      <c r="BR60" s="9"/>
+      <c r="BS60" s="9"/>
+      <c r="BT60" s="10"/>
     </row>
     <row r="62" spans="4:72" x14ac:dyDescent="0.2">
-      <c r="E62" s="8"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
-      <c r="P62" s="9"/>
-      <c r="Q62" s="9"/>
-      <c r="R62" s="9"/>
-      <c r="S62" s="9"/>
-      <c r="T62" s="9"/>
-      <c r="U62" s="9"/>
-      <c r="V62" s="9"/>
-      <c r="W62" s="9"/>
-      <c r="X62" s="9"/>
-      <c r="Y62" s="9"/>
-      <c r="Z62" s="9"/>
-      <c r="AA62" s="9"/>
-      <c r="AB62" s="9"/>
-      <c r="AC62" s="9"/>
-      <c r="AD62" s="9"/>
-      <c r="AE62" s="9"/>
-      <c r="AF62" s="9"/>
-      <c r="AG62" s="9"/>
-      <c r="AH62" s="9"/>
-      <c r="AI62" s="9"/>
-      <c r="AJ62" s="9"/>
-      <c r="AK62" s="9"/>
-      <c r="AL62" s="9"/>
-      <c r="AM62" s="9"/>
-      <c r="AN62" s="9"/>
-      <c r="AO62" s="9"/>
-      <c r="AP62" s="9"/>
-      <c r="AQ62" s="9"/>
-      <c r="AR62" s="9"/>
-      <c r="AS62" s="9"/>
-      <c r="AT62" s="9"/>
-      <c r="AU62" s="9"/>
-      <c r="AV62" s="9"/>
-      <c r="AW62" s="9"/>
-      <c r="AX62" s="9"/>
-      <c r="AY62" s="9"/>
-      <c r="AZ62" s="9"/>
-      <c r="BA62" s="9"/>
-      <c r="BB62" s="9"/>
-      <c r="BC62" s="9"/>
-      <c r="BD62" s="9"/>
-      <c r="BE62" s="9"/>
-      <c r="BF62" s="9"/>
-      <c r="BG62" s="9"/>
-      <c r="BH62" s="9"/>
-      <c r="BI62" s="9"/>
-      <c r="BJ62" s="9"/>
-      <c r="BK62" s="9"/>
-      <c r="BL62" s="9"/>
-      <c r="BM62" s="9"/>
-      <c r="BN62" s="9"/>
-      <c r="BO62" s="9"/>
-      <c r="BP62" s="9"/>
-      <c r="BQ62" s="9"/>
-      <c r="BR62" s="9"/>
-      <c r="BS62" s="9"/>
-      <c r="BT62" s="10"/>
-    </row>
-    <row r="64" spans="4:72" x14ac:dyDescent="0.2">
-      <c r="D64" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="4:72" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="4:72" x14ac:dyDescent="0.2">
+      <c r="G64" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="4:30" x14ac:dyDescent="0.2">
@@ -8623,15 +8435,15 @@
         <v>43</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="4:30" x14ac:dyDescent="0.2">
+      <c r="F66" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="G66" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="4:30" x14ac:dyDescent="0.2">
@@ -8639,7 +8451,7 @@
         <v>43</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="4:30" x14ac:dyDescent="0.2">
@@ -8647,31 +8459,31 @@
         <v>43</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="F69" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="F70" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G70" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="G71" s="1" t="s">
+    <row r="69" spans="4:30" x14ac:dyDescent="0.2">
+      <c r="G69" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H69" s="1" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="4:30" x14ac:dyDescent="0.2">
+      <c r="D70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="4:30" x14ac:dyDescent="0.2">
+      <c r="D71" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="4:30" x14ac:dyDescent="0.2">
@@ -8679,274 +8491,222 @@
         <v>37</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="73" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="D73" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="D74" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E74" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F76" s="24" t="s">
+    <row r="73" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F74" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13" t="s">
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="P74" s="14"/>
+      <c r="Q74" s="14"/>
+      <c r="R74" s="14"/>
+      <c r="S74" s="14"/>
+      <c r="T74" s="14"/>
+      <c r="U74" s="14"/>
+      <c r="V74" s="14"/>
+      <c r="W74" s="14"/>
+      <c r="X74" s="14"/>
+      <c r="Y74" s="14"/>
+      <c r="Z74" s="14"/>
+      <c r="AA74" s="14"/>
+      <c r="AB74" s="14"/>
+      <c r="AC74" s="14"/>
+      <c r="AD74" s="21"/>
+    </row>
+    <row r="75" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F75" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="P75" s="22"/>
+      <c r="Q75" s="22"/>
+      <c r="R75" s="22"/>
+      <c r="S75" s="22"/>
+      <c r="T75" s="22"/>
+      <c r="U75" s="22"/>
+      <c r="V75" s="22"/>
+      <c r="W75" s="22"/>
+      <c r="X75" s="22"/>
+      <c r="Y75" s="22"/>
+      <c r="Z75" s="22"/>
+      <c r="AA75" s="22"/>
+      <c r="AB75" s="22"/>
+      <c r="AC75" s="22"/>
+      <c r="AD75" s="23"/>
+    </row>
+    <row r="76" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F76" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
+      <c r="K76" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L76" s="19"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+      <c r="O76" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="P76" s="22"/>
+      <c r="Q76" s="22"/>
+      <c r="R76" s="22"/>
+      <c r="S76" s="22"/>
+      <c r="T76" s="22"/>
+      <c r="U76" s="22"/>
+      <c r="V76" s="22"/>
+      <c r="W76" s="22"/>
+      <c r="X76" s="22"/>
+      <c r="Y76" s="22"/>
+      <c r="Z76" s="22"/>
+      <c r="AA76" s="22"/>
+      <c r="AB76" s="22"/>
+      <c r="AC76" s="22"/>
+      <c r="AD76" s="23"/>
+    </row>
+    <row r="77" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F77" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L77" s="19"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
+      <c r="O77" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="P77" s="22"/>
+      <c r="Q77" s="22"/>
+      <c r="R77" s="22"/>
+      <c r="S77" s="22"/>
+      <c r="T77" s="22"/>
+      <c r="U77" s="22"/>
+      <c r="V77" s="22"/>
+      <c r="W77" s="22"/>
+      <c r="X77" s="22"/>
+      <c r="Y77" s="22"/>
+      <c r="Z77" s="22"/>
+      <c r="AA77" s="22"/>
+      <c r="AB77" s="22"/>
+      <c r="AC77" s="22"/>
+      <c r="AD77" s="23"/>
+    </row>
+    <row r="78" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F78" s="15">
+        <v>6</v>
+      </c>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
+      <c r="K78" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L78" s="19"/>
+      <c r="M78" s="19"/>
+      <c r="N78" s="19"/>
+      <c r="O78" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="13"/>
-      <c r="S76" s="13"/>
-      <c r="T76" s="13"/>
-      <c r="U76" s="13"/>
-      <c r="V76" s="13"/>
-      <c r="W76" s="13"/>
-      <c r="X76" s="13"/>
-      <c r="Y76" s="13"/>
-      <c r="Z76" s="13"/>
-      <c r="AA76" s="13"/>
-      <c r="AB76" s="13"/>
-      <c r="AC76" s="13"/>
-      <c r="AD76" s="17"/>
-    </row>
-    <row r="77" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="F77" s="25">
-        <v>0</v>
-      </c>
-      <c r="G77" s="26"/>
-      <c r="H77" s="26"/>
-      <c r="I77" s="26"/>
-      <c r="J77" s="26"/>
-      <c r="K77" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="L77" s="14"/>
-      <c r="M77" s="14"/>
-      <c r="N77" s="14"/>
-      <c r="O77" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="18"/>
-      <c r="S77" s="18"/>
-      <c r="T77" s="18"/>
-      <c r="U77" s="18"/>
-      <c r="V77" s="18"/>
-      <c r="W77" s="18"/>
-      <c r="X77" s="18"/>
-      <c r="Y77" s="18"/>
-      <c r="Z77" s="18"/>
-      <c r="AA77" s="18"/>
-      <c r="AB77" s="18"/>
-      <c r="AC77" s="18"/>
-      <c r="AD77" s="19"/>
-    </row>
-    <row r="78" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F78" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="G78" s="28"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="28"/>
-      <c r="K78" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="P78" s="20"/>
-      <c r="Q78" s="20"/>
-      <c r="R78" s="20"/>
-      <c r="S78" s="20"/>
-      <c r="T78" s="20"/>
-      <c r="U78" s="20"/>
-      <c r="V78" s="20"/>
-      <c r="W78" s="20"/>
-      <c r="X78" s="20"/>
-      <c r="Y78" s="20"/>
-      <c r="Z78" s="20"/>
-      <c r="AA78" s="20"/>
-      <c r="AB78" s="20"/>
-      <c r="AC78" s="20"/>
-      <c r="AD78" s="21"/>
-    </row>
-    <row r="79" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F79" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G79" s="28"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28"/>
-      <c r="K79" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="15"/>
-      <c r="O79" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="P79" s="20"/>
-      <c r="Q79" s="20"/>
-      <c r="R79" s="20"/>
-      <c r="S79" s="20"/>
-      <c r="T79" s="20"/>
-      <c r="U79" s="20"/>
-      <c r="V79" s="20"/>
-      <c r="W79" s="20"/>
-      <c r="X79" s="20"/>
-      <c r="Y79" s="20"/>
-      <c r="Z79" s="20"/>
-      <c r="AA79" s="20"/>
-      <c r="AB79" s="20"/>
-      <c r="AC79" s="20"/>
-      <c r="AD79" s="21"/>
-    </row>
-    <row r="80" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F80" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="G80" s="28"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
-      <c r="K80" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="P80" s="20"/>
-      <c r="Q80" s="20"/>
-      <c r="R80" s="20"/>
-      <c r="S80" s="20"/>
-      <c r="T80" s="20"/>
-      <c r="U80" s="20"/>
-      <c r="V80" s="20"/>
-      <c r="W80" s="20"/>
-      <c r="X80" s="20"/>
-      <c r="Y80" s="20"/>
-      <c r="Z80" s="20"/>
-      <c r="AA80" s="20"/>
-      <c r="AB80" s="20"/>
-      <c r="AC80" s="20"/>
-      <c r="AD80" s="21"/>
-    </row>
-    <row r="81" spans="6:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F81" s="27">
-        <v>7</v>
-      </c>
-      <c r="G81" s="28"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
-      <c r="K81" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="P81" s="20"/>
-      <c r="Q81" s="20"/>
-      <c r="R81" s="20"/>
-      <c r="S81" s="20"/>
-      <c r="T81" s="20"/>
-      <c r="U81" s="20"/>
-      <c r="V81" s="20"/>
-      <c r="W81" s="20"/>
-      <c r="X81" s="20"/>
-      <c r="Y81" s="20"/>
-      <c r="Z81" s="20"/>
-      <c r="AA81" s="20"/>
-      <c r="AB81" s="20"/>
-      <c r="AC81" s="20"/>
-      <c r="AD81" s="21"/>
-    </row>
-    <row r="82" spans="6:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F82" s="22"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="23"/>
-      <c r="K82" s="16"/>
-      <c r="L82" s="16"/>
-      <c r="M82" s="16"/>
-      <c r="N82" s="16"/>
-      <c r="O82" s="11"/>
-      <c r="P82" s="11"/>
-      <c r="Q82" s="11"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="11"/>
-      <c r="T82" s="11"/>
-      <c r="U82" s="11"/>
-      <c r="V82" s="11"/>
-      <c r="W82" s="11"/>
-      <c r="X82" s="11"/>
-      <c r="Y82" s="11"/>
-      <c r="Z82" s="11"/>
-      <c r="AA82" s="11"/>
-      <c r="AB82" s="11"/>
-      <c r="AC82" s="11"/>
-      <c r="AD82" s="12"/>
+      <c r="P78" s="22"/>
+      <c r="Q78" s="22"/>
+      <c r="R78" s="22"/>
+      <c r="S78" s="22"/>
+      <c r="T78" s="22"/>
+      <c r="U78" s="22"/>
+      <c r="V78" s="22"/>
+      <c r="W78" s="22"/>
+      <c r="X78" s="22"/>
+      <c r="Y78" s="22"/>
+      <c r="Z78" s="22"/>
+      <c r="AA78" s="22"/>
+      <c r="AB78" s="22"/>
+      <c r="AC78" s="22"/>
+      <c r="AD78" s="23"/>
+    </row>
+    <row r="79" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="11"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="20"/>
+      <c r="L79" s="20"/>
+      <c r="M79" s="20"/>
+      <c r="N79" s="20"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="17"/>
+      <c r="R79" s="17"/>
+      <c r="S79" s="17"/>
+      <c r="T79" s="17"/>
+      <c r="U79" s="17"/>
+      <c r="V79" s="17"/>
+      <c r="W79" s="17"/>
+      <c r="X79" s="17"/>
+      <c r="Y79" s="17"/>
+      <c r="Z79" s="17"/>
+      <c r="AA79" s="17"/>
+      <c r="AB79" s="17"/>
+      <c r="AC79" s="17"/>
+      <c r="AD79" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="F82:J82"/>
-    <mergeCell ref="F76:J76"/>
-    <mergeCell ref="F77:J77"/>
-    <mergeCell ref="F78:J78"/>
-    <mergeCell ref="F79:J79"/>
-    <mergeCell ref="F80:J80"/>
-    <mergeCell ref="F81:J81"/>
-    <mergeCell ref="O82:AD82"/>
+  <mergeCells count="18">
+    <mergeCell ref="O79:AD79"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
     <mergeCell ref="K76:N76"/>
     <mergeCell ref="K77:N77"/>
     <mergeCell ref="K78:N78"/>
     <mergeCell ref="K79:N79"/>
-    <mergeCell ref="K80:N80"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="K82:N82"/>
+    <mergeCell ref="O74:AD74"/>
+    <mergeCell ref="O75:AD75"/>
     <mergeCell ref="O76:AD76"/>
     <mergeCell ref="O77:AD77"/>
     <mergeCell ref="O78:AD78"/>
-    <mergeCell ref="O79:AD79"/>
-    <mergeCell ref="O80:AD80"/>
-    <mergeCell ref="O81:AD81"/>
+    <mergeCell ref="F79:J79"/>
+    <mergeCell ref="F74:J74"/>
+    <mergeCell ref="F75:J75"/>
+    <mergeCell ref="F76:J76"/>
+    <mergeCell ref="F77:J77"/>
+    <mergeCell ref="F78:J78"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8958,7 +8718,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:BT51"/>
+  <dimension ref="B2:BT54"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -11570,74 +11330,284 @@
       <c r="BT50" s="7"/>
     </row>
     <row r="51" spans="5:72" x14ac:dyDescent="0.2">
-      <c r="E51" s="8"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
-      <c r="Q51" s="9"/>
-      <c r="R51" s="9"/>
-      <c r="S51" s="9"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
-      <c r="V51" s="9"/>
-      <c r="W51" s="9"/>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="9"/>
-      <c r="Z51" s="9"/>
-      <c r="AA51" s="9"/>
-      <c r="AB51" s="9"/>
-      <c r="AC51" s="9"/>
-      <c r="AD51" s="9"/>
-      <c r="AE51" s="9"/>
-      <c r="AF51" s="9"/>
-      <c r="AG51" s="9"/>
-      <c r="AH51" s="9"/>
-      <c r="AI51" s="9"/>
-      <c r="AJ51" s="9"/>
-      <c r="AK51" s="9"/>
-      <c r="AL51" s="9"/>
-      <c r="AM51" s="9"/>
-      <c r="AN51" s="9"/>
-      <c r="AO51" s="9"/>
-      <c r="AP51" s="9"/>
-      <c r="AQ51" s="9"/>
-      <c r="AR51" s="9"/>
-      <c r="AS51" s="9"/>
-      <c r="AT51" s="9"/>
-      <c r="AU51" s="9"/>
-      <c r="AV51" s="9"/>
-      <c r="AW51" s="9"/>
-      <c r="AX51" s="9"/>
-      <c r="AY51" s="9"/>
-      <c r="AZ51" s="9"/>
-      <c r="BA51" s="9"/>
-      <c r="BB51" s="9"/>
-      <c r="BC51" s="9"/>
-      <c r="BD51" s="9"/>
-      <c r="BE51" s="9"/>
-      <c r="BF51" s="9"/>
-      <c r="BG51" s="9"/>
-      <c r="BH51" s="9"/>
-      <c r="BI51" s="9"/>
-      <c r="BJ51" s="9"/>
-      <c r="BK51" s="9"/>
-      <c r="BL51" s="9"/>
-      <c r="BM51" s="9"/>
-      <c r="BN51" s="9"/>
-      <c r="BO51" s="9"/>
-      <c r="BP51" s="9"/>
-      <c r="BQ51" s="9"/>
-      <c r="BR51" s="9"/>
-      <c r="BS51" s="9"/>
-      <c r="BT51" s="10"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="6"/>
+      <c r="T51" s="6"/>
+      <c r="U51" s="6"/>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="6"/>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="6"/>
+      <c r="AE51" s="6"/>
+      <c r="AF51" s="6"/>
+      <c r="AG51" s="6"/>
+      <c r="AH51" s="6"/>
+      <c r="AI51" s="6"/>
+      <c r="AJ51" s="6"/>
+      <c r="AK51" s="6"/>
+      <c r="AL51" s="6"/>
+      <c r="AM51" s="6"/>
+      <c r="AN51" s="6"/>
+      <c r="AO51" s="6"/>
+      <c r="AP51" s="6"/>
+      <c r="AQ51" s="6"/>
+      <c r="AR51" s="6"/>
+      <c r="AS51" s="6"/>
+      <c r="AT51" s="6"/>
+      <c r="AU51" s="6"/>
+      <c r="AV51" s="6"/>
+      <c r="AW51" s="6"/>
+      <c r="AX51" s="6"/>
+      <c r="AY51" s="6"/>
+      <c r="AZ51" s="6"/>
+      <c r="BA51" s="6"/>
+      <c r="BB51" s="6"/>
+      <c r="BC51" s="6"/>
+      <c r="BD51" s="6"/>
+      <c r="BE51" s="6"/>
+      <c r="BF51" s="6"/>
+      <c r="BG51" s="6"/>
+      <c r="BH51" s="6"/>
+      <c r="BI51" s="6"/>
+      <c r="BJ51" s="6"/>
+      <c r="BK51" s="6"/>
+      <c r="BL51" s="6"/>
+      <c r="BM51" s="6"/>
+      <c r="BN51" s="6"/>
+      <c r="BO51" s="6"/>
+      <c r="BP51" s="6"/>
+      <c r="BQ51" s="6"/>
+      <c r="BR51" s="6"/>
+      <c r="BS51" s="6"/>
+      <c r="BT51" s="7"/>
+    </row>
+    <row r="52" spans="5:72" x14ac:dyDescent="0.2">
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="6"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="6"/>
+      <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="6"/>
+      <c r="AB52" s="6"/>
+      <c r="AC52" s="6"/>
+      <c r="AD52" s="6"/>
+      <c r="AE52" s="6"/>
+      <c r="AF52" s="6"/>
+      <c r="AG52" s="6"/>
+      <c r="AH52" s="6"/>
+      <c r="AI52" s="6"/>
+      <c r="AJ52" s="6"/>
+      <c r="AK52" s="6"/>
+      <c r="AL52" s="6"/>
+      <c r="AM52" s="6"/>
+      <c r="AN52" s="6"/>
+      <c r="AO52" s="6"/>
+      <c r="AP52" s="6"/>
+      <c r="AQ52" s="6"/>
+      <c r="AR52" s="6"/>
+      <c r="AS52" s="6"/>
+      <c r="AT52" s="6"/>
+      <c r="AU52" s="6"/>
+      <c r="AV52" s="6"/>
+      <c r="AW52" s="6"/>
+      <c r="AX52" s="6"/>
+      <c r="AY52" s="6"/>
+      <c r="AZ52" s="6"/>
+      <c r="BA52" s="6"/>
+      <c r="BB52" s="6"/>
+      <c r="BC52" s="6"/>
+      <c r="BD52" s="6"/>
+      <c r="BE52" s="6"/>
+      <c r="BF52" s="6"/>
+      <c r="BG52" s="6"/>
+      <c r="BH52" s="6"/>
+      <c r="BI52" s="6"/>
+      <c r="BJ52" s="6"/>
+      <c r="BK52" s="6"/>
+      <c r="BL52" s="6"/>
+      <c r="BM52" s="6"/>
+      <c r="BN52" s="6"/>
+      <c r="BO52" s="6"/>
+      <c r="BP52" s="6"/>
+      <c r="BQ52" s="6"/>
+      <c r="BR52" s="6"/>
+      <c r="BS52" s="6"/>
+      <c r="BT52" s="7"/>
+    </row>
+    <row r="53" spans="5:72" x14ac:dyDescent="0.2">
+      <c r="E53" s="5"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="6"/>
+      <c r="AA53" s="6"/>
+      <c r="AB53" s="6"/>
+      <c r="AC53" s="6"/>
+      <c r="AD53" s="6"/>
+      <c r="AE53" s="6"/>
+      <c r="AF53" s="6"/>
+      <c r="AG53" s="6"/>
+      <c r="AH53" s="6"/>
+      <c r="AI53" s="6"/>
+      <c r="AJ53" s="6"/>
+      <c r="AK53" s="6"/>
+      <c r="AL53" s="6"/>
+      <c r="AM53" s="6"/>
+      <c r="AN53" s="6"/>
+      <c r="AO53" s="6"/>
+      <c r="AP53" s="6"/>
+      <c r="AQ53" s="6"/>
+      <c r="AR53" s="6"/>
+      <c r="AS53" s="6"/>
+      <c r="AT53" s="6"/>
+      <c r="AU53" s="6"/>
+      <c r="AV53" s="6"/>
+      <c r="AW53" s="6"/>
+      <c r="AX53" s="6"/>
+      <c r="AY53" s="6"/>
+      <c r="AZ53" s="6"/>
+      <c r="BA53" s="6"/>
+      <c r="BB53" s="6"/>
+      <c r="BC53" s="6"/>
+      <c r="BD53" s="6"/>
+      <c r="BE53" s="6"/>
+      <c r="BF53" s="6"/>
+      <c r="BG53" s="6"/>
+      <c r="BH53" s="6"/>
+      <c r="BI53" s="6"/>
+      <c r="BJ53" s="6"/>
+      <c r="BK53" s="6"/>
+      <c r="BL53" s="6"/>
+      <c r="BM53" s="6"/>
+      <c r="BN53" s="6"/>
+      <c r="BO53" s="6"/>
+      <c r="BP53" s="6"/>
+      <c r="BQ53" s="6"/>
+      <c r="BR53" s="6"/>
+      <c r="BS53" s="6"/>
+      <c r="BT53" s="7"/>
+    </row>
+    <row r="54" spans="5:72" x14ac:dyDescent="0.2">
+      <c r="E54" s="8"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="9"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="9"/>
+      <c r="AI54" s="9"/>
+      <c r="AJ54" s="9"/>
+      <c r="AK54" s="9"/>
+      <c r="AL54" s="9"/>
+      <c r="AM54" s="9"/>
+      <c r="AN54" s="9"/>
+      <c r="AO54" s="9"/>
+      <c r="AP54" s="9"/>
+      <c r="AQ54" s="9"/>
+      <c r="AR54" s="9"/>
+      <c r="AS54" s="9"/>
+      <c r="AT54" s="9"/>
+      <c r="AU54" s="9"/>
+      <c r="AV54" s="9"/>
+      <c r="AW54" s="9"/>
+      <c r="AX54" s="9"/>
+      <c r="AY54" s="9"/>
+      <c r="AZ54" s="9"/>
+      <c r="BA54" s="9"/>
+      <c r="BB54" s="9"/>
+      <c r="BC54" s="9"/>
+      <c r="BD54" s="9"/>
+      <c r="BE54" s="9"/>
+      <c r="BF54" s="9"/>
+      <c r="BG54" s="9"/>
+      <c r="BH54" s="9"/>
+      <c r="BI54" s="9"/>
+      <c r="BJ54" s="9"/>
+      <c r="BK54" s="9"/>
+      <c r="BL54" s="9"/>
+      <c r="BM54" s="9"/>
+      <c r="BN54" s="9"/>
+      <c r="BO54" s="9"/>
+      <c r="BP54" s="9"/>
+      <c r="BQ54" s="9"/>
+      <c r="BR54" s="9"/>
+      <c r="BS54" s="9"/>
+      <c r="BT54" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Update slave data. -Update design of data format used to communicate with other device via SPI. -Add and update code to communicate to send rotation, as RPM, and velocity of wheel.
</commit_message>
<xml_diff>
--- a/dev/doc/sequence_design.xlsx
+++ b/dev/doc/sequence_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="日付更新" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
     <sheet name="ライト点灯状態_更新(手動の場合)" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">回転数_速度_更新!$B$2:$E$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">回転数_速度_更新!$F$74:$F$79</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -753,10 +753,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>LSB = 0.01[km/h]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>H/Wには、Arduino nano互換の中華版を使用する。</t>
     <rPh sb="18" eb="20">
       <t>ゴカン</t>
@@ -867,15 +863,25 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>0～1</t>
+    <t>LSB = 0.001[km/h]</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2～3</t>
+    <t>開始</t>
+    <rPh sb="0" eb="2">
+      <t>カイシ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>4～5</t>
+    <t>終了</t>
+    <rPh sb="0" eb="2">
+      <t>シュウリョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>サイズ</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -928,7 +934,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1023,51 +1029,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -1107,9 +1068,94 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1122,10 +1168,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -1137,16 +1194,46 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1155,7 +1242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1167,37 +1254,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2650,8 +2734,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>70</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>71</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>12121</xdr:rowOff>
     </xdr:to>
@@ -3173,7 +3257,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:BV41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5403,15 +5487,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:BT79"/>
+  <dimension ref="B2:BT80"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU73" sqref="AU73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="2" style="1"/>
-    <col min="9" max="9" width="2.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="2" style="1"/>
+    <col min="1" max="16384" width="2" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
@@ -8430,7 +8514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:31" x14ac:dyDescent="0.2">
       <c r="F65" s="1" t="s">
         <v>43</v>
       </c>
@@ -8438,7 +8522,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:31" x14ac:dyDescent="0.2">
       <c r="F66" s="1" t="s">
         <v>43</v>
       </c>
@@ -8446,7 +8530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:31" x14ac:dyDescent="0.2">
       <c r="F67" s="1" t="s">
         <v>43</v>
       </c>
@@ -8454,7 +8538,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:31" x14ac:dyDescent="0.2">
       <c r="F68" s="1" t="s">
         <v>43</v>
       </c>
@@ -8462,89 +8546,90 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:31" x14ac:dyDescent="0.2">
       <c r="G69" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="70" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:31" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="71" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:31" x14ac:dyDescent="0.2">
       <c r="D71" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="72" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:31" x14ac:dyDescent="0.2">
       <c r="D72" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="4:31" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F74" s="26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="73" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F74" s="13" t="s">
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M74" s="20"/>
+      <c r="N74" s="20"/>
+      <c r="O74" s="20"/>
+      <c r="P74" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L74" s="14"/>
-      <c r="M74" s="14"/>
-      <c r="N74" s="14"/>
-      <c r="O74" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="P74" s="14"/>
-      <c r="Q74" s="14"/>
-      <c r="R74" s="14"/>
-      <c r="S74" s="14"/>
-      <c r="T74" s="14"/>
-      <c r="U74" s="14"/>
-      <c r="V74" s="14"/>
-      <c r="W74" s="14"/>
-      <c r="X74" s="14"/>
-      <c r="Y74" s="14"/>
-      <c r="Z74" s="14"/>
-      <c r="AA74" s="14"/>
-      <c r="AB74" s="14"/>
-      <c r="AC74" s="14"/>
-      <c r="AD74" s="21"/>
-    </row>
-    <row r="75" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F75" s="15" t="s">
+      <c r="Q74" s="20"/>
+      <c r="R74" s="20"/>
+      <c r="S74" s="20"/>
+      <c r="T74" s="20"/>
+      <c r="U74" s="20"/>
+      <c r="V74" s="20"/>
+      <c r="W74" s="20"/>
+      <c r="X74" s="20"/>
+      <c r="Y74" s="20"/>
+      <c r="Z74" s="20"/>
+      <c r="AA74" s="20"/>
+      <c r="AB74" s="20"/>
+      <c r="AC74" s="20"/>
+      <c r="AD74" s="20"/>
+      <c r="AE74" s="21"/>
+    </row>
+    <row r="75" spans="4:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F75" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="19" t="s">
-        <v>59</v>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22" t="s">
+        <v>65</v>
       </c>
-      <c r="L75" s="19"/>
-      <c r="M75" s="19"/>
-      <c r="N75" s="19"/>
-      <c r="O75" s="22" t="s">
-        <v>61</v>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22" t="s">
+        <v>66</v>
       </c>
+      <c r="K75" s="22"/>
+      <c r="L75" s="22"/>
+      <c r="M75" s="22"/>
+      <c r="N75" s="22"/>
+      <c r="O75" s="22"/>
       <c r="P75" s="22"/>
       <c r="Q75" s="22"/>
       <c r="R75" s="22"/>
@@ -8559,119 +8644,152 @@
       <c r="AA75" s="22"/>
       <c r="AB75" s="22"/>
       <c r="AC75" s="22"/>
-      <c r="AD75" s="23"/>
-    </row>
-    <row r="76" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F76" s="15" t="s">
-        <v>65</v>
+      <c r="AD75" s="22"/>
+      <c r="AE75" s="23"/>
+    </row>
+    <row r="76" spans="4:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F76" s="25">
+        <v>0</v>
       </c>
-      <c r="G76" s="16"/>
-      <c r="H76" s="16"/>
-      <c r="I76" s="16"/>
-      <c r="J76" s="16"/>
-      <c r="K76" s="19" t="s">
+      <c r="G76" s="18"/>
+      <c r="H76" s="16">
+        <f>F76+J76-1</f>
+        <v>3</v>
+      </c>
+      <c r="I76" s="18"/>
+      <c r="J76" s="16">
+        <v>4</v>
+      </c>
+      <c r="K76" s="18"/>
+      <c r="L76" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="18"/>
+      <c r="P76" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q76" s="17"/>
+      <c r="R76" s="17"/>
+      <c r="S76" s="17"/>
+      <c r="T76" s="17"/>
+      <c r="U76" s="17"/>
+      <c r="V76" s="17"/>
+      <c r="W76" s="17"/>
+      <c r="X76" s="17"/>
+      <c r="Y76" s="17"/>
+      <c r="Z76" s="17"/>
+      <c r="AA76" s="17"/>
+      <c r="AB76" s="17"/>
+      <c r="AC76" s="17"/>
+      <c r="AD76" s="17"/>
+      <c r="AE76" s="19"/>
+    </row>
+    <row r="77" spans="4:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F77" s="25">
+        <f>H76+1</f>
+        <v>4</v>
+      </c>
+      <c r="G77" s="18"/>
+      <c r="H77" s="16">
+        <f t="shared" ref="H77:H79" si="0">F77+J77-1</f>
+        <v>7</v>
+      </c>
+      <c r="I77" s="18"/>
+      <c r="J77" s="16">
+        <v>4</v>
+      </c>
+      <c r="K77" s="18"/>
+      <c r="L77" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="18"/>
+      <c r="P77" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q77" s="17"/>
+      <c r="R77" s="17"/>
+      <c r="S77" s="17"/>
+      <c r="T77" s="17"/>
+      <c r="U77" s="17"/>
+      <c r="V77" s="17"/>
+      <c r="W77" s="17"/>
+      <c r="X77" s="17"/>
+      <c r="Y77" s="17"/>
+      <c r="Z77" s="17"/>
+      <c r="AA77" s="17"/>
+      <c r="AB77" s="17"/>
+      <c r="AC77" s="17"/>
+      <c r="AD77" s="17"/>
+      <c r="AE77" s="19"/>
+    </row>
+    <row r="78" spans="4:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F78" s="25">
+        <f t="shared" ref="F78:F79" si="1">H77+1</f>
+        <v>8</v>
+      </c>
+      <c r="G78" s="18"/>
+      <c r="H78" s="16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I78" s="18"/>
+      <c r="J78" s="16">
+        <v>4</v>
+      </c>
+      <c r="K78" s="18"/>
+      <c r="L78" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q78" s="17"/>
+      <c r="R78" s="17"/>
+      <c r="S78" s="17"/>
+      <c r="T78" s="17"/>
+      <c r="U78" s="17"/>
+      <c r="V78" s="17"/>
+      <c r="W78" s="17"/>
+      <c r="X78" s="17"/>
+      <c r="Y78" s="17"/>
+      <c r="Z78" s="17"/>
+      <c r="AA78" s="17"/>
+      <c r="AB78" s="17"/>
+      <c r="AC78" s="17"/>
+      <c r="AD78" s="17"/>
+      <c r="AE78" s="19"/>
+    </row>
+    <row r="79" spans="4:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F79" s="25">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G79" s="18"/>
+      <c r="H79" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I79" s="18"/>
+      <c r="J79" s="16">
+        <v>1</v>
+      </c>
+      <c r="K79" s="18"/>
+      <c r="L79" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="18"/>
+      <c r="P79" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L76" s="19"/>
-      <c r="M76" s="19"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="P76" s="22"/>
-      <c r="Q76" s="22"/>
-      <c r="R76" s="22"/>
-      <c r="S76" s="22"/>
-      <c r="T76" s="22"/>
-      <c r="U76" s="22"/>
-      <c r="V76" s="22"/>
-      <c r="W76" s="22"/>
-      <c r="X76" s="22"/>
-      <c r="Y76" s="22"/>
-      <c r="Z76" s="22"/>
-      <c r="AA76" s="22"/>
-      <c r="AB76" s="22"/>
-      <c r="AC76" s="22"/>
-      <c r="AD76" s="23"/>
-    </row>
-    <row r="77" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F77" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
-      <c r="I77" s="16"/>
-      <c r="J77" s="16"/>
-      <c r="K77" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="L77" s="19"/>
-      <c r="M77" s="19"/>
-      <c r="N77" s="19"/>
-      <c r="O77" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="P77" s="22"/>
-      <c r="Q77" s="22"/>
-      <c r="R77" s="22"/>
-      <c r="S77" s="22"/>
-      <c r="T77" s="22"/>
-      <c r="U77" s="22"/>
-      <c r="V77" s="22"/>
-      <c r="W77" s="22"/>
-      <c r="X77" s="22"/>
-      <c r="Y77" s="22"/>
-      <c r="Z77" s="22"/>
-      <c r="AA77" s="22"/>
-      <c r="AB77" s="22"/>
-      <c r="AC77" s="22"/>
-      <c r="AD77" s="23"/>
-    </row>
-    <row r="78" spans="4:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F78" s="15">
-        <v>6</v>
-      </c>
-      <c r="G78" s="16"/>
-      <c r="H78" s="16"/>
-      <c r="I78" s="16"/>
-      <c r="J78" s="16"/>
-      <c r="K78" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="L78" s="19"/>
-      <c r="M78" s="19"/>
-      <c r="N78" s="19"/>
-      <c r="O78" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="P78" s="22"/>
-      <c r="Q78" s="22"/>
-      <c r="R78" s="22"/>
-      <c r="S78" s="22"/>
-      <c r="T78" s="22"/>
-      <c r="U78" s="22"/>
-      <c r="V78" s="22"/>
-      <c r="W78" s="22"/>
-      <c r="X78" s="22"/>
-      <c r="Y78" s="22"/>
-      <c r="Z78" s="22"/>
-      <c r="AA78" s="22"/>
-      <c r="AB78" s="22"/>
-      <c r="AC78" s="22"/>
-      <c r="AD78" s="23"/>
-    </row>
-    <row r="79" spans="4:30" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F79" s="11"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
-      <c r="K79" s="20"/>
-      <c r="L79" s="20"/>
-      <c r="M79" s="20"/>
-      <c r="N79" s="20"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
       <c r="Q79" s="17"/>
       <c r="R79" s="17"/>
       <c r="S79" s="17"/>
@@ -8685,28 +8803,70 @@
       <c r="AA79" s="17"/>
       <c r="AB79" s="17"/>
       <c r="AC79" s="17"/>
-      <c r="AD79" s="18"/>
+      <c r="AD79" s="17"/>
+      <c r="AE79" s="19"/>
+    </row>
+    <row r="80" spans="4:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F80" s="14"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="11"/>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="13"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="12"/>
+      <c r="R80" s="12"/>
+      <c r="S80" s="12"/>
+      <c r="T80" s="12"/>
+      <c r="U80" s="12"/>
+      <c r="V80" s="12"/>
+      <c r="W80" s="12"/>
+      <c r="X80" s="12"/>
+      <c r="Y80" s="12"/>
+      <c r="Z80" s="12"/>
+      <c r="AA80" s="12"/>
+      <c r="AB80" s="12"/>
+      <c r="AC80" s="12"/>
+      <c r="AD80" s="12"/>
+      <c r="AE80" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="O79:AD79"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K79:N79"/>
-    <mergeCell ref="O74:AD74"/>
-    <mergeCell ref="O75:AD75"/>
-    <mergeCell ref="O76:AD76"/>
-    <mergeCell ref="O77:AD77"/>
-    <mergeCell ref="O78:AD78"/>
-    <mergeCell ref="F79:J79"/>
-    <mergeCell ref="F74:J74"/>
-    <mergeCell ref="F75:J75"/>
-    <mergeCell ref="F76:J76"/>
-    <mergeCell ref="F77:J77"/>
-    <mergeCell ref="F78:J78"/>
+  <mergeCells count="31">
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F74:K74"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="P74:AE75"/>
+    <mergeCell ref="L74:O75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="L76:O76"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="L78:O78"/>
+    <mergeCell ref="L79:O79"/>
+    <mergeCell ref="P76:AE76"/>
+    <mergeCell ref="P77:AE77"/>
+    <mergeCell ref="P78:AE78"/>
+    <mergeCell ref="P79:AE79"/>
+    <mergeCell ref="L77:O77"/>
+    <mergeCell ref="L80:O80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="P80:AE80"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>